<commit_message>
Add method for calculating diagonal of futures at expiration. Excel implementation.
</commit_message>
<xml_diff>
--- a/xllfms/tlmm.xlsx
+++ b/xllfms/tlmm.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keith\Source\Repos\libfms\xllfms\"/>
@@ -15,11 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -96,6 +91,1170 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$9:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.455501782733191E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7357922206277032E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7357922206277032E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7357922206277032E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$10:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.455501782733191E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7357922206277032E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.039315394658622E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.039315394658622E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$11:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.455501782733191E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7357922206277032E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.039315394658622E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5074515607196691E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$12:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="292173592"/>
+        <c:axId val="292173984"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="292173592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="292173984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="292173984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="292173592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -361,10 +1520,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M12"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B2:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,7 +1534,7 @@
     <col min="4" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -394,7 +1554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -414,7 +1574,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -434,7 +1594,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -472,35 +1632,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>_xll.CURVE.LMM.RESET(B8)</f>
+        <v>1.5469165943444789E-225</v>
+      </c>
       <c r="C7">
         <f>C2</f>
         <v>1</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:G7" si="0">D2</f>
+        <f>D2</f>
         <v>2</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>E2</f>
         <v>3</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f>F2</f>
         <v>4</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>G2</f>
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0</v>
-      </c>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>_xll.CURVE.LMM(C2:G2, C3:G3, C4:G4, B5, D5:M5)</f>
-        <v>1.9886710030439084E-191</v>
+        <v>1.5469165943444789E-225</v>
       </c>
       <c r="C8" s="3">
         <f t="array" ref="C8:G8">_xll.CURVE.LMM.FORWARD(B8)</f>
@@ -519,107 +1680,105 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <f>_xll.CURVE.LMM.TO(B8, A9)</f>
-        <v>1.9886710030439084E-191</v>
+        <f>_xll.DEPENDS(_xll.CURVE.LMM.NEXT(B8),C8:G8)</f>
+        <v>1.5469165943444789E-225</v>
       </c>
       <c r="C9" s="3">
         <f t="array" ref="C9:G9">_xll.CURVE.LMM.FORWARD(B9)</f>
         <v>0.02</v>
       </c>
       <c r="D9" s="3">
-        <v>1.7134605244429231E-2</v>
+        <v>1.8983301595898682E-2</v>
       </c>
       <c r="E9" s="3">
-        <v>2.3539644770515455E-2</v>
+        <v>1.7987403668095443E-2</v>
       </c>
       <c r="F9" s="3">
-        <v>2.3539644770515455E-2</v>
+        <v>1.7987403668095443E-2</v>
       </c>
       <c r="G9" s="3">
-        <v>2.3539644770515455E-2</v>
+        <v>1.7987403668095443E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <f>_xll.CURVE.LMM.TO(B9, A10)</f>
-        <v>1.9886710030439084E-191</v>
+        <f>_xll.DEPENDS(_xll.CURVE.LMM.NEXT(B9),C9:G9)</f>
+        <v>1.5469165943444789E-225</v>
       </c>
       <c r="C10" s="3">
         <f t="array" ref="C10:G10">_xll.CURVE.LMM.FORWARD(B10)</f>
         <v>0.02</v>
       </c>
       <c r="D10" s="3">
-        <v>1.7134605244429231E-2</v>
+        <v>1.8983301595898682E-2</v>
       </c>
       <c r="E10" s="3">
-        <v>2.1431959721944786E-2</v>
+        <v>1.7987403668095443E-2</v>
       </c>
       <c r="F10" s="3">
-        <v>2.093661786409547E-2</v>
+        <v>1.6884312598303194E-2</v>
       </c>
       <c r="G10" s="3">
-        <v>2.2788200072776821E-2</v>
+        <v>1.6884312598303194E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>3</v>
-      </c>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <f>_xll.CURVE.LMM.TO(B10, A11)</f>
-        <v>1.9886710030439084E-191</v>
+        <f>_xll.DEPENDS(_xll.CURVE.LMM.NEXT(B10),C10:G10)</f>
+        <v>1.5469165943444789E-225</v>
       </c>
       <c r="C11" s="3">
         <f t="array" ref="C11:G11">_xll.CURVE.LMM.FORWARD(B11)</f>
         <v>0.02</v>
       </c>
       <c r="D11" s="3">
-        <v>1.7134605244429231E-2</v>
+        <v>1.8983301595898682E-2</v>
       </c>
       <c r="E11" s="3">
-        <v>2.1431959721944786E-2</v>
+        <v>1.7987403668095443E-2</v>
       </c>
       <c r="F11" s="3">
-        <v>2.093661786409547E-2</v>
+        <v>1.6884312598303194E-2</v>
       </c>
       <c r="G11" s="3">
-        <v>2.2788200072776821E-2</v>
+        <v>1.4921955611935231E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>4</v>
-      </c>
-      <c r="B12" s="2">
-        <f>_xll.CURVE.LMM.TO(B11, A12)</f>
-        <v>1.9886710030439084E-191</v>
-      </c>
-      <c r="C12" s="3">
-        <f t="array" ref="C12:G12">_xll.CURVE.LMM.FORWARD(B12)</f>
-        <v>0.02</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1.7134605244429231E-2</v>
-      </c>
-      <c r="E12" s="3">
-        <v>2.1431959721944786E-2</v>
-      </c>
-      <c r="F12" s="3">
-        <v>2.093661786409547E-2</v>
-      </c>
-      <c r="G12" s="3">
-        <v>2.2788200072776821E-2</v>
-      </c>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!J9:J15</xm:f>
+              <xm:sqref>K9</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>